<commit_message>
[BUG] Fix bug with hours
</commit_message>
<xml_diff>
--- a/EDT_EAH/bin/Debug/TEMPLATE.xlsx
+++ b/EDT_EAH/bin/Debug/TEMPLATE.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\edt-eah\EDT_EAH\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Perso\edt-eah\EDT_EAH\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E11838-F3A5-48C7-882A-C2F18BDFBFD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -32,61 +33,16 @@
     <t>Chambre</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>14h15</t>
   </si>
   <si>
     <t>15h00</t>
   </si>
-  <si>
-    <t>HDJ 1</t>
-  </si>
-  <si>
-    <t>HDJ 2</t>
-  </si>
-  <si>
-    <t>HDJ 3</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-40C]dddd\ d\ mmmm\ yyyy"/>
   </numFmts>
@@ -563,23 +519,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A3" sqref="A3:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" style="4" customWidth="1"/>
-    <col min="4" max="8" width="18.453125" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="18.28515625" style="4" customWidth="1"/>
+    <col min="4" max="8" width="18.42578125" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -587,7 +543,7 @@
         <v>44095</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -612,16 +568,14 @@
         <v>11h45</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="12"/>
       <c r="D3" s="13"/>
@@ -630,10 +584,8 @@
       <c r="G3" s="13"/>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="15"/>
       <c r="D4" s="16"/>
@@ -642,10 +594,8 @@
       <c r="G4" s="16"/>
       <c r="H4" s="17"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>4</v>
-      </c>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
@@ -654,10 +604,8 @@
       <c r="G5" s="13"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>5</v>
-      </c>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="15"/>
       <c r="D6" s="16"/>
@@ -666,10 +614,8 @@
       <c r="G6" s="16"/>
       <c r="H6" s="17"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>6</v>
-      </c>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
@@ -678,10 +624,8 @@
       <c r="G7" s="13"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>7</v>
-      </c>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -690,10 +634,8 @@
       <c r="G8" s="16"/>
       <c r="H8" s="17"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>8</v>
-      </c>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
@@ -702,10 +644,8 @@
       <c r="G9" s="13"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
-        <v>9</v>
-      </c>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
@@ -714,10 +654,8 @@
       <c r="G10" s="16"/>
       <c r="H10" s="17"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
-        <v>10</v>
-      </c>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="12"/>
       <c r="D11" s="13"/>
@@ -726,10 +664,8 @@
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>11</v>
-      </c>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
@@ -738,10 +674,8 @@
       <c r="G12" s="16"/>
       <c r="H12" s="17"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
-        <v>12</v>
-      </c>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
@@ -750,10 +684,8 @@
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
-        <v>13</v>
-      </c>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
@@ -762,10 +694,8 @@
       <c r="G14" s="16"/>
       <c r="H14" s="17"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
-        <v>16</v>
-      </c>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
@@ -774,10 +704,8 @@
       <c r="G15" s="13"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>17</v>
-      </c>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
@@ -786,10 +714,8 @@
       <c r="G16" s="16"/>
       <c r="H16" s="17"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
-        <v>18</v>
-      </c>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="12"/>
       <c r="D17" s="18"/>
@@ -798,10 +724,10 @@
       <c r="G17" s="18"/>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" s="11"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
     </row>
   </sheetData>

</xml_diff>